<commit_message>
Update CSSECDV - Case Study 2 Access Matrix.xlsx
</commit_message>
<xml_diff>
--- a/Case Study 2/CSSECDV - Case Study 2 Access Matrix.xlsx
+++ b/Case Study 2/CSSECDV - Case Study 2 Access Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ejose\Documents\Github\CSSECDV\Case Study 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DFC592-B354-4592-B50C-4165436E1343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5C2FDA-6CEC-42D6-B078-5C146AC7D10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="161">
   <si>
     <t>ACCESS MATRIX</t>
   </si>
@@ -420,9 +420,6 @@
     <t>1. Database (User Data &amp; Logs)
 2. java.security - Hashing
 3. java.security - Encryption</t>
-  </si>
-  <si>
-    <t>Requires Admin user to enter PW</t>
   </si>
   <si>
     <t>1. JPasswordField - Admin Password
@@ -552,6 +549,12 @@
   <si>
     <t>1. Attempted logout will be recorded.
 2. Session will be set to null or no value.</t>
+  </si>
+  <si>
+    <t>1. Only Admin users are allowed to access debug mode.</t>
+  </si>
+  <si>
+    <t>Requires Admin user to enter PW to make changes.</t>
   </si>
 </sst>
 </file>
@@ -1167,9 +1170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CZ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="175" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="175" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1254,7 @@
         <v>126</v>
       </c>
       <c r="Q2" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R2" s="25" t="s">
         <v>14</v>
@@ -1634,7 +1637,7 @@
         <v>124</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>123</v>
@@ -1686,7 +1689,7 @@
         <v>124</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>123</v>
@@ -1736,7 +1739,7 @@
         <v>124</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>123</v>
@@ -1784,7 +1787,7 @@
         <v>124</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>123</v>
@@ -1798,16 +1801,16 @@
         <v>120</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>120</v>
@@ -1816,7 +1819,7 @@
         <v>120</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="3"/>
@@ -2018,17 +2021,17 @@
         <v>101</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>131</v>
-      </c>
       <c r="F10" s="5" t="s">
         <v>120</v>
       </c>
@@ -2036,29 +2039,31 @@
         <v>120</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>120</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="N10" s="5"/>
+        <v>149</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="O10" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q10" s="5" t="s">
         <v>120</v>
@@ -2159,49 +2164,49 @@
         <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="P11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:104" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2209,52 +2214,52 @@
         <v>103</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
@@ -2349,52 +2354,52 @@
         <v>104</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="O13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:104" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2404,7 +2409,7 @@
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -2516,7 +2521,7 @@
         <v>107</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>106</v>
@@ -2537,10 +2542,10 @@
         <v>120</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>120</v>
@@ -2552,7 +2557,7 @@
         <v>120</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>120</v>

</xml_diff>